<commit_message>
various changes including edition of repeater
</commit_message>
<xml_diff>
--- a/changes to knaus.xlsx
+++ b/changes to knaus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\AppData\Roaming\talon\user\kronenfeld_talon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E69E7D2-B593-4B5D-B139-73B882AFA027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210693C7-2E17-40E2-91B8-744B5ED33D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{6CF8A999-8755-4369-985F-C16916B38D26}"/>
+    <workbookView xWindow="10834" yWindow="0" windowWidth="11109" windowHeight="11623" activeTab="3" xr2:uid="{6CF8A999-8755-4369-985F-C16916B38D26}"/>
   </bookViews>
   <sheets>
     <sheet name="app_name_overrides" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Folder</t>
   </si>
@@ -198,6 +198,30 @@
   </si>
   <si>
     <t>notepad++.exe</t>
+  </si>
+  <si>
+    <t>126-129</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>added comma_separated format to formatters dictionary</t>
+  </si>
+  <si>
+    <t>added karma spoken phrase for comma_separated formatter</t>
+  </si>
+  <si>
+    <t>core/keys</t>
+  </si>
+  <si>
+    <t>keys.py</t>
+  </si>
+  <si>
+    <t>forward delete</t>
+  </si>
+  <si>
+    <t>flick</t>
   </si>
 </sst>
 </file>
@@ -566,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A06F9E1-B60C-4308-A447-249DE19A495B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
@@ -729,10 +753,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BB0897-B843-4E24-BFDC-47A235709CBE}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -843,6 +867,60 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>147</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>257</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>